<commit_message>
Add IS second year subjects
</commit_message>
<xml_diff>
--- a/is-gradings.xlsx
+++ b/is-gradings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DASUN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raminduwalgama/Documents/Projects/uni_ranker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB4DC71-0C18-4909-9973-CD8639502CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD97F36-5BE6-A149-8C6C-62C75EA5BF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="subject_info" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>Data Structures and Algorithms I</t>
   </si>
@@ -243,13 +243,19 @@
   </si>
   <si>
     <t>IS 2114</t>
+  </si>
+  <si>
+    <t>IS 2102</t>
+  </si>
+  <si>
+    <t>Group Project I</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -260,10 +266,12 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1608,22 +1616,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.36328125" defaultRowHeight="20" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.36328125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.36328125" style="1"/>
+    <col min="3" max="3" width="7.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" customHeight="1">
+    <row r="1" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -1634,7 +1642,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20.25" customHeight="1">
+    <row r="2" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>48</v>
       </c>
@@ -1645,7 +1653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20" customHeight="1">
+    <row r="3" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>49</v>
       </c>
@@ -1656,7 +1664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20" customHeight="1">
+    <row r="4" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>50</v>
       </c>
@@ -1667,7 +1675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20" customHeight="1">
+    <row r="5" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>51</v>
       </c>
@@ -1678,7 +1686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20" customHeight="1">
+    <row r="6" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>52</v>
       </c>
@@ -1689,7 +1697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="20" customHeight="1">
+    <row r="7" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>53</v>
       </c>
@@ -1700,7 +1708,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20" customHeight="1">
+    <row r="8" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>54</v>
       </c>
@@ -1711,7 +1719,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20" customHeight="1">
+    <row r="9" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>46</v>
       </c>
@@ -1722,7 +1730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="20" customHeight="1">
+    <row r="10" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>47</v>
       </c>
@@ -1733,7 +1741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="20" customHeight="1">
+    <row r="11" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>55</v>
       </c>
@@ -1744,7 +1752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20" customHeight="1">
+    <row r="12" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>56</v>
       </c>
@@ -1755,7 +1763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20" customHeight="1">
+    <row r="13" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>57</v>
       </c>
@@ -1766,7 +1774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="20" customHeight="1">
+    <row r="14" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>58</v>
       </c>
@@ -1777,7 +1785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="20" customHeight="1">
+    <row r="15" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>59</v>
       </c>
@@ -1788,7 +1796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="20" customHeight="1">
+    <row r="16" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>60</v>
       </c>
@@ -1799,7 +1807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="20" customHeight="1">
+    <row r="17" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>61</v>
       </c>
@@ -1810,18 +1818,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="20" customHeight="1">
+    <row r="18" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="C18" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="20" customHeight="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
         <v>62</v>
       </c>
@@ -1829,10 +1837,10 @@
         <v>35</v>
       </c>
       <c r="C19" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="20" customHeight="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
         <v>63</v>
       </c>
@@ -1843,7 +1851,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="20" customHeight="1">
+    <row r="21" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
         <v>64</v>
       </c>
@@ -1851,10 +1859,10 @@
         <v>37</v>
       </c>
       <c r="C21" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="20" customHeight="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
         <v>65</v>
       </c>
@@ -1865,80 +1873,91 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="20" customHeight="1">
+    <row r="23" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C23" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="20" customHeight="1">
+    <row r="24" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C25" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="20" customHeight="1">
-      <c r="A25" s="3" t="s">
+    <row r="26" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B26" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C26" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="20" customHeight="1">
-      <c r="A26" s="3" t="s">
+    <row r="27" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B27" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C27" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="20" customHeight="1">
-      <c r="A27" s="3" t="s">
+    <row r="28" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B28" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="C27" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="20" customHeight="1">
-      <c r="A28" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="C28" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="20" customHeight="1">
+    <row r="29" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B30" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C30" s="7">
         <v>2</v>
       </c>
     </row>
@@ -1966,13 +1985,13 @@
       <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.36328125" defaultRowHeight="20" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="3" width="16.36328125" style="8" customWidth="1"/>
-    <col min="4" max="16384" width="16.36328125" style="8"/>
+    <col min="1" max="3" width="16.33203125" style="8" customWidth="1"/>
+    <col min="4" max="16384" width="16.33203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.25" customHeight="1">
+    <row r="1" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -1980,7 +1999,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="20.25" customHeight="1">
+    <row r="2" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>7</v>
       </c>
@@ -1988,7 +2007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20" customHeight="1">
+    <row r="3" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
@@ -1996,7 +2015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="20" customHeight="1">
+    <row r="4" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
         <v>9</v>
       </c>
@@ -2004,7 +2023,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="20" customHeight="1">
+    <row r="5" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>10</v>
       </c>
@@ -2012,7 +2031,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="20" customHeight="1">
+    <row r="6" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
         <v>11</v>
       </c>
@@ -2020,7 +2039,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="20" customHeight="1">
+    <row r="7" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>12</v>
       </c>
@@ -2028,7 +2047,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="20" customHeight="1">
+    <row r="8" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>13</v>
       </c>
@@ -2036,7 +2055,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="20" customHeight="1">
+    <row r="9" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>14</v>
       </c>
@@ -2044,7 +2063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="20" customHeight="1">
+    <row r="10" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
@@ -2052,7 +2071,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="20" customHeight="1">
+    <row r="11" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
         <v>16</v>
       </c>
@@ -2060,7 +2079,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="20" customHeight="1">
+    <row r="12" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
         <v>17</v>
       </c>
@@ -2068,7 +2087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="20" customHeight="1">
+    <row r="13" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
         <v>18</v>
       </c>
@@ -2076,7 +2095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="20" customHeight="1">
+    <row r="14" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="12" t="s">
         <v>19</v>
       </c>

</xml_diff>